<commit_message>
add more benchmark data
</commit_message>
<xml_diff>
--- a/results/benchmark_report.xlsx
+++ b/results/benchmark_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,17 +528,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1x6000</t>
+          <t>2x4090</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2008.1</v>
+        <v>467.26</v>
       </c>
       <c r="C6" t="n">
-        <v>1.29</v>
+        <v>0.78</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1784439685938616</v>
+        <v>0.4636961577422991</v>
       </c>
     </row>
     <row r="7">
@@ -548,13 +548,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4752.34</v>
+        <v>4556.7</v>
       </c>
       <c r="C7" t="n">
         <v>0.78</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0455915752380231</v>
+        <v>0.04754903036554232</v>
       </c>
     </row>
     <row r="8">
@@ -564,61 +564,93 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>8052.43</v>
+        <v>1230.14</v>
       </c>
       <c r="C8" t="n">
         <v>1.3</v>
       </c>
       <c r="D8" t="n">
-        <v>0.04484498606148841</v>
+        <v>0.2935528566757533</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4x4090</t>
+          <t>2x5090</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8998.370000000001</v>
+        <v>8411.16</v>
       </c>
       <c r="C9" t="n">
-        <v>1.56</v>
+        <v>1.3</v>
       </c>
       <c r="D9" t="n">
-        <v>0.04815686989236198</v>
+        <v>0.04293237925697658</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4x5090</t>
+          <t>4x4090</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>8460.450000000001</v>
+        <v>8902.5</v>
       </c>
       <c r="C10" t="n">
-        <v>2.6</v>
+        <v>1.56</v>
       </c>
       <c r="D10" t="n">
-        <v>0.08536451633450019</v>
+        <v>0.04867546569315735</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>4x4090</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>906.1900000000001</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.4781925791868519</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>4x4090</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1731.44</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.2502733755332748</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>4x5090</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>2486.72</v>
-      </c>
-      <c r="C11" t="n">
+      <c r="B13" t="n">
+        <v>2501.38</v>
+      </c>
+      <c r="C13" t="n">
         <v>2.6</v>
       </c>
-      <c r="D11" t="n">
-        <v>0.2904316618767783</v>
+      <c r="D13" t="n">
+        <v>0.2887295101992589</v>
       </c>
     </row>
   </sheetData>

</xml_diff>